<commit_message>
Resolvido o problema da importação cricular
</commit_message>
<xml_diff>
--- a/Codigos/SRC/clientes.xlsx
+++ b/Codigos/SRC/clientes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,6 +467,57 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>18026822-a885-43a8-884a-3682ab6bf9bd</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Marcos</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>joaovitorbatista12337@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>cb783894-e9a6-4eee-887a-d9dbeca80720</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Joaquim</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>email.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2b800868-aa5c-4131-b8c8-d0fd4e56494d</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>VemPAo</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Pao@gmail.com</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>